<commit_message>
Sync from silver-sycamore 2026-01-12
</commit_message>
<xml_diff>
--- a/content/artifacts/silver-sycamore-master.xlsx
+++ b/content/artifacts/silver-sycamore-master.xlsx
@@ -22,6 +22,7 @@
     <sheet name="DOCUMENTS" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="INITIATIVES" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="REFERENCE" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="PACKAGE_DETAILS" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -31,7 +32,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -64,8 +65,12 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -76,6 +81,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="001F4E79"/>
         <bgColor rgb="001F4E79"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -107,6 +118,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -495,11 +514,10 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Last updated: 2026-01-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="3"/>
+          <t>Last updated: 2026-01-10</t>
+        </is>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
@@ -580,41 +598,46 @@
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <f>HYPERLINK("#EVENT_PACKAGES!A2", "EVENT_PACKAGES (11)")</f>
+        <f>HYPERLINK("#FORMS!A2", "FORMS (5)")</f>
         <v/>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Event Packages: 11</t>
+          <t>Forms: 5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4">
-        <f>HYPERLINK("#CATERING!A2", "CATERING (9)")</f>
+        <f>HYPERLINK("#CATERING!A2", "CATERING (6)")</f>
         <v/>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Catering Menus: 9</t>
+          <t>Catering Packages: 6</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4">
-        <f>HYPERLINK("#BAR!A2", "BAR (10)")</f>
+        <f>HYPERLINK("#ADD_ONS!A2", "ADD_ONS (14)")</f>
         <v/>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Add-On Services: 33</t>
+          <t>Add-ons: 14</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4">
-        <f>HYPERLINK("#ADD_ONS!A2", "ADD_ONS (33)")</f>
+        <f>HYPERLINK("#PACKAGE_DETAILS!A2", "PACKAGE_DETAILS")</f>
         <v/>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Detailed package information</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -652,7 +675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,25 +745,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cash Bar</t>
+          <t>Open Bar (50 guests)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>675</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
+        <v>1150</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Bartender + officer</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Guests pay $5/drink</t>
+          <t>Bartender + officer, domestic beer/wine</t>
         </is>
       </c>
     </row>
@@ -752,21 +768,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Open Bar (50 guests)</t>
+          <t>Open Bar (100 guests)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1175</v>
+        <v>1675</v>
       </c>
       <c r="D5" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Bartender + officer, domestic beer/wine</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -776,21 +791,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Open Bar (100 guests)</t>
+          <t>Cash Bar</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1675</v>
-      </c>
-      <c r="D6" t="n">
-        <v>100</v>
+        <v>675</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bartender + officer, domestic beer/wine</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>Bartender + officer</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Guests pay $5/drink</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -806,11 +827,14 @@
       <c r="C7" t="n">
         <v>15</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Additional capacity</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Add-on</t>
+          <t>Add-on for open bar</t>
         </is>
       </c>
     </row>
@@ -822,13 +846,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Liquor setups</t>
+          <t>Liquor Setups</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>4.5</v>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Sodas/juices</t>
@@ -848,121 +871,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Afternoon Cash Bar</t>
+          <t>Mimosa Bar</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>175</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+        <v>15</v>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1 bartender</t>
+          <t>3 juices, 3 fruits, Moscato</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Guests pay $5/drink</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>BAR-007</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Evening Cash Bar</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>675</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1 bartender + officer</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>BAR-008</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Small Party Bartender</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>150</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Beer, wine, mimosas</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>$5/drink</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>BAR-009</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Mimosa Bar</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>15</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>3 juices, 3 fruits, Moscato</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Per person, ~2 drinks</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>BAR-010</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Bucket of Beer (jail)</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>10</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>~2 beers/person</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Per person</t>
+          <t>Popular brunch option</t>
         </is>
       </c>
     </row>
@@ -977,7 +899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,23 +969,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Early Bridal Cottage Access (10am)</t>
+          <t>Queso Fountain</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>500</v>
+        <v>7.5</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>flat</t>
+          <t>per person</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Venue</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>100 guest minimum</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1103,25 +1029,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bucket of Beer (jail)</t>
+          <t>Early Bridal Cottage Access (10am)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>per person</t>
+          <t>flat</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bar</t>
+          <t>Venue</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>~2 beers/person</t>
+          <t>Early access for bride prep</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1077,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Your name on it</t>
+          <t>Personalized welcome sign</t>
         </is>
       </c>
     </row>
@@ -1163,11 +1089,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Saloon Rental (additional)</t>
+          <t>Dance Floor</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1176,10 +1102,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Venue</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Equipment</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12x15, outdoor street</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1189,11 +1119,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Saloon Rental (with alcohol)</t>
+          <t>Photo Booth</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>650</v>
+        <v>250</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1202,12 +1132,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Venue</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Discounted, up to $1600</t>
+          <t>Entertainment</t>
         </is>
       </c>
     </row>
@@ -1219,11 +1144,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dance Floor (small)</t>
+          <t>Yard Games</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>750</v>
+        <v>1350</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1232,12 +1157,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Equipment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>12x15, street</t>
+          <t>Complete set</t>
         </is>
       </c>
     </row>
@@ -1249,11 +1174,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Dance Floor (large)</t>
+          <t>Open Bar (50 guests)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1262,10 +1187,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Equipment</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>Bar</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Bartender + officer, beer/wine</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1275,11 +1204,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Photo Booth</t>
+          <t>Open Bar (100 guests)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>750</v>
+        <v>1675</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1288,12 +1217,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Bar</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Attendant, props, backdrop, USB</t>
+          <t>Bartender + officer, beer/wine</t>
         </is>
       </c>
     </row>
@@ -1305,11 +1234,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Photo Booth (3hr, banquet)</t>
+          <t>Cash Bar</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>550</v>
+        <v>675</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1318,10 +1247,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>Bar</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Guests pay $5/drink, includes officer</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1331,23 +1264,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Personalized Town Cake Gazebo</t>
+          <t>Bucket of Beer (jail)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>flat</t>
+          <t>per person</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Decor</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
+          <t>Bar</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>~2 beers/person</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1357,11 +1294,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Harpist</t>
+          <t>Liquor Setups</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1370,10 +1307,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>Bar</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Sodas/juices, guest-supplied liquor</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1383,11 +1324,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Popcorn Machine + attendant</t>
+          <t>Saloon Rental (additional)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1396,10 +1337,9 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
+          <t>Venue</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1409,11 +1349,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mechanical Bull (4 hrs)</t>
+          <t>Saloon Rental (with alcohol)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1350</v>
+        <v>650</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1422,566 +1362,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Venue</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Verified $1350</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ADD-015</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Yard Games</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>200</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Cornhole, Jenga, Tic Tac Toe, horseshoes</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ADD-016</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Yard Games (wedding)</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>1350</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Premium package</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ADD-017</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>B&amp;B Package</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Lodging</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>8 rooms, 16 guests, $1200-1600</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ADD-018</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Additional Hours</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Venue</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Only 1 additional hour</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>ADD-019</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>DJ Package</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>687.5</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>$575-$800 range</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>ADD-020</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Dueling Pianos/Acoustic</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>700</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>1 hour, +$275/additional</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>ADD-021</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Queso Fountain</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Min 100, 2hr service</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>ADD-022</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Decorated Tiered Cake</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Plus delivery fee</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>ADD-023</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Cake cutting/plating</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Client supplies cake</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>ADD-024</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Dessert add-on (banquet)</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>4</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Choice of 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>ADD-025</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Grilled Asparagus</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>ADD-026</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Shrimp Scampi (pasta)</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>3</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>ADD-027</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Add Chicken (Texas Tradition)</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>5</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>ADD-028</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Plated service (vs buffet)</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>4</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>per person</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Catering</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>ADD-029</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Silver Sycamore Decor Add-On</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>75</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Decor</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Consultation + setup/cleanup</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>ADD-030</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Linen Color Upgrade</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>15</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>per table</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Decor</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Non-white options</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>ADD-031</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Balloon Arch (8-16ft)</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>192.5</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Decor</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>$135-250 range</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>ADD-032</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Balloon Garland (school)</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>185</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Decor</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>School colors</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>ADD-033</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Uplighting (signature)</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>flat</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Decor</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>White, pink, red</t>
+          <t>Discounted rate, up to $1600</t>
         </is>
       </c>
     </row>
@@ -1996,7 +1382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2050,6 +1436,16 @@
           <t>Event Type</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Fees</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2077,6 +1473,11 @@
           <t>Wedding</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Primary wedding contract form</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2086,22 +1487,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Shower/Party Booking Form</t>
+          <t>Tasting Appointment Form</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Showers, small parties</t>
+          <t>Menu tastings</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Guest of honor, event type, cake, bar, menu</t>
+          <t>Party name, date, guest count</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Shower/Party</t>
+          <t>Tasting</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Free for 2 people</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>$10/extra person, $50 late cancellation</t>
         </is>
       </c>
     </row>
@@ -2113,22 +1524,91 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Shower/Small Party Booking Form</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Showers, small parties</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Guest of honor, event type, cake, bar, menu</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Shower/Party</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Initial booking form</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FRM-004</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Shower/Small Party Contract</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Showers, small parties</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Full contract details</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Shower/Party</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Contract version of shower form</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FRM-005</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Corporate Booking Form</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Business events</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Company name, responsible party, event type, guest count</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Corporate</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Uses wedding contract template</t>
         </is>
       </c>
     </row>
@@ -3097,7 +2577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3105,7 +2585,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3121,7 +2606,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
@@ -3157,7 +2641,6 @@
         </is>
       </c>
     </row>
-    <row r="9"/>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
@@ -3193,7 +2676,6 @@
         </is>
       </c>
     </row>
-    <row r="15"/>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
@@ -3229,7 +2711,6 @@
         </is>
       </c>
     </row>
-    <row r="21"/>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
@@ -3248,6 +2729,830 @@
       <c r="A24" t="inlineStr">
         <is>
           <t>(281) 487-4033</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9" t="inlineStr">
+        <is>
+          <t>WEDDING PACKAGE COMPARISON</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>Best For</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>Price Range</t>
+        </is>
+      </c>
+      <c r="D28" s="10" t="inlineStr">
+        <is>
+          <t>Guest Count</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="F28" s="10" t="inlineStr">
+        <is>
+          <t>Key Features</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>Dream Package</t>
+        </is>
+      </c>
+      <c r="B29" s="8" t="inlineStr">
+        <is>
+          <t>Full weddings 100+ guests</t>
+        </is>
+      </c>
+      <c r="C29" s="8" t="inlineStr">
+        <is>
+          <t>$12,900</t>
+        </is>
+      </c>
+      <c r="D29" s="8" t="inlineStr">
+        <is>
+          <t>100+</t>
+        </is>
+      </c>
+      <c r="E29" s="8" t="inlineStr">
+        <is>
+          <t>5 hrs</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="inlineStr">
+        <is>
+          <t>Ceremony + reception, all spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>Reception Only</t>
+        </is>
+      </c>
+      <c r="B30" s="8" t="inlineStr">
+        <is>
+          <t>Ceremony elsewhere</t>
+        </is>
+      </c>
+      <c r="C30" s="8" t="inlineStr">
+        <is>
+          <t>$11,400</t>
+        </is>
+      </c>
+      <c r="D30" s="8" t="inlineStr">
+        <is>
+          <t>100+</t>
+        </is>
+      </c>
+      <c r="E30" s="8" t="inlineStr">
+        <is>
+          <t>4 hrs</t>
+        </is>
+      </c>
+      <c r="F30" s="8" t="inlineStr">
+        <is>
+          <t>Reception hall only</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>Simple Elegance</t>
+        </is>
+      </c>
+      <c r="B31" s="8" t="inlineStr">
+        <is>
+          <t>Mid-size weddings</t>
+        </is>
+      </c>
+      <c r="C31" s="8" t="inlineStr">
+        <is>
+          <t>$7,800-$8,800</t>
+        </is>
+      </c>
+      <c r="D31" s="8" t="inlineStr">
+        <is>
+          <t>50+</t>
+        </is>
+      </c>
+      <c r="E31" s="8" t="inlineStr">
+        <is>
+          <t>3.5 hrs</t>
+        </is>
+      </c>
+      <c r="F31" s="8" t="inlineStr">
+        <is>
+          <t>Ceremony + reception, smaller</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>Micro Wedding</t>
+        </is>
+      </c>
+      <c r="B32" s="8" t="inlineStr">
+        <is>
+          <t>Intimate gatherings</t>
+        </is>
+      </c>
+      <c r="C32" s="8" t="inlineStr">
+        <is>
+          <t>$3,200-$4,200</t>
+        </is>
+      </c>
+      <c r="D32" s="8" t="inlineStr">
+        <is>
+          <t>20+</t>
+        </is>
+      </c>
+      <c r="E32" s="8" t="inlineStr">
+        <is>
+          <t>2.5 hrs</t>
+        </is>
+      </c>
+      <c r="F32" s="8" t="inlineStr">
+        <is>
+          <t>Saloon &amp; Town spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="9" t="inlineStr">
+        <is>
+          <t>CATERING PACKAGES</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="10" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>Price/Person</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>Style</t>
+        </is>
+      </c>
+      <c r="D37" s="10" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>All the Possibilities</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>$22</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Buffet</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Pasta-focused options</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Sycamore Comfort</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>$25</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Buffet</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Chicken entrees</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Texas Tradition</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>$27</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Buffet</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>BBQ brisket + sausage</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Tex Mex Party Time</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>$35</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Buffet</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Fajitas + queso fountain</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Gold Dinner</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>$39</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Buffet/Plated</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Premium options</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Platinum Dinner</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>$44</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Plated</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Top tier, dual entrees</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="9" t="inlineStr">
+        <is>
+          <t>POPULAR ADD-ONS</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="10" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B48" s="10" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C48" s="10" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Open Bar (50)</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>$1,150</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Includes bartender + officer</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Open Bar (100)</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>$1,675</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Includes bartender + officer</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Cash Bar</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>$675</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Guests pay $5/drink</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Queso Fountain</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>$7.50/person</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>100 guest minimum</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Mimosa Bar</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>$15/person</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>3 juices, 3 fruits, Moscato</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Dance Floor</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>$750</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>12x15 outdoor</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Photo Booth</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>$250</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Entertainment</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Yard Games</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>$1,350</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Complete set</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Early Cottage Access</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>$500</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Bridal prep from 10am</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Town Sign</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>$175</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Personalized welcome</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="9" t="inlineStr">
+        <is>
+          <t>BOOKING FORMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="10" t="inlineStr">
+        <is>
+          <t>Form</t>
+        </is>
+      </c>
+      <c r="B63" s="10" t="inlineStr">
+        <is>
+          <t>Purpose</t>
+        </is>
+      </c>
+      <c r="C63" s="10" t="inlineStr">
+        <is>
+          <t>Special Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Wedding Booking Form</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Full weddings</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Primary contract</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Tasting Appointment</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Menu tastings</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Free for 2, $10/extra, $50 late cancel</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Shower/Party Booking</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Showers &amp; small events</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Initial form</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Shower/Party Contract</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Showers &amp; small events</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Contract version</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Corporate Booking</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Business events</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Uses wedding contract template</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1">
+        <f>HYPERLINK("#DASHBOARD!A1", "← Dashboard")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Package</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Price Range</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>Guests</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>What's Included</t>
+        </is>
+      </c>
+      <c r="F3" s="6" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>Dream Package</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>$12,900</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="inlineStr">
+        <is>
+          <t>100 guests</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>5 hours</t>
+        </is>
+      </c>
+      <c r="E4" s="8" t="inlineStr">
+        <is>
+          <t>Ceremony + Reception, Main hall, White chapel, Bridal cottage, Groom jail prep area</t>
+        </is>
+      </c>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>$20/person over 100, $2000 deposit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>Simple Elegance</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="inlineStr">
+        <is>
+          <t>$7,800 (Mon-Thu) / $8,800 (Fri-Sun)</t>
+        </is>
+      </c>
+      <c r="C5" s="8" t="inlineStr">
+        <is>
+          <t>50 guests</t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t>3.5 hours</t>
+        </is>
+      </c>
+      <c r="E5" s="8" t="inlineStr">
+        <is>
+          <t>Ceremony + Reception, Venue spaces, Basic setup</t>
+        </is>
+      </c>
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>$35/person over 50, Weekday discount available</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>Reception Only</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="inlineStr">
+        <is>
+          <t>$11,400</t>
+        </is>
+      </c>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>100 guests</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>4 hours</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
+        <is>
+          <t>Reception hall only, No ceremony spaces</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>$20/person over 100, $2000 deposit</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>Micro Wedding</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="inlineStr">
+        <is>
+          <t>$3,200 (Mon-Thu) / $4,200 (Fri-Sun)</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>20 guests</t>
+        </is>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>2.5 hours</t>
+        </is>
+      </c>
+      <c r="E7" s="8" t="inlineStr">
+        <is>
+          <t>Saloon &amp; Town spaces, Intimate setting</t>
+        </is>
+      </c>
+      <c r="F7" s="8" t="inlineStr">
+        <is>
+          <t>$35/person over 20, $1500 deposit</t>
         </is>
       </c>
     </row>
@@ -3354,14 +3659,11 @@
           <t>Utility</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>1tearoom</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>Active</t>
@@ -3483,7 +3785,6 @@
           <t>Sycamoreville29</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>Active</t>
@@ -3563,7 +3864,6 @@
           <t>1tearoom</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>Active</t>
@@ -3586,7 +3886,6 @@
           <t>Booking</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>silversycamore</t>
@@ -3597,7 +3896,6 @@
           <t>1tearoom</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>Active</t>
@@ -3746,7 +4044,6 @@
           <t>Marketing</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
           <t>658731</t>
@@ -3826,7 +4123,6 @@
           <t>Marketing</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -3948,13 +4244,11 @@
           <t>Utility</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
           <t>admin@Silversycamore.com</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
           <t>Utility</t>
@@ -3982,7 +4276,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
           <t>12344</t>
@@ -3993,7 +4286,6 @@
           <t>sycamoreville</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4016,7 +4308,6 @@
           <t>Utility</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
           <t>silversycamore</t>
@@ -4054,7 +4345,6 @@
           <t>Utility</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
           <t>jms@spigener.com</t>
@@ -4176,7 +4466,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -4187,7 +4476,6 @@
           <t>Sycamoreville211</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4210,7 +4498,6 @@
           <t>Utility</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -4221,7 +4508,6 @@
           <t>1tearoom</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4301,7 +4587,6 @@
           <t>Jackie1town11</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4381,7 +4666,6 @@
           <t>571212</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4419,7 +4703,6 @@
           <t>Sycamoreville11</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4442,7 +4725,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -4453,7 +4735,6 @@
           <t>Silvertraining19</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4476,7 +4757,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
           <t>jms@spigener.com</t>
@@ -4487,7 +4767,6 @@
           <t>Sycamoreville22!</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4510,7 +4789,6 @@
           <t>Storage</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
           <t>silversycamoreweddings@gmail.com</t>
@@ -4521,7 +4799,6 @@
           <t>Sycamoreville211</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4722,8 +4999,6 @@
           <t>silversycamore</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
           <t>Active</t>
@@ -4751,7 +5026,6 @@
           <t>groupon.com</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
           <t>Silvertown19!</t>
@@ -4784,8 +5058,6 @@
           <t>Utility</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
           <t>spiqco travel12345</t>
@@ -4860,13 +5132,11 @@
           <t>Booking</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
           <t>18948306</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
           <t>Property ID</t>
@@ -4904,7 +5174,6 @@
           <t>admin@silversycamore.com</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
           <t>Hardware</t>
@@ -4932,7 +5201,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
           <t>kayla</t>
@@ -4943,7 +5211,6 @@
           <t>IDL0822</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
           <t>Active</t>
@@ -5050,7 +5317,6 @@
           <t>Device</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -5088,7 +5354,6 @@
           <t>Security</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
           <t>silversycamoreweddings@gmail.com</t>
@@ -5178,8 +5443,6 @@
           <t>admin@silversycamore.com</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
           <t>Active</t>
@@ -5212,7 +5475,6 @@
           <t>jms@spigener.com</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
           <t>Alt email</t>
@@ -5240,7 +5502,6 @@
           <t>Booking</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -5251,7 +5512,6 @@
           <t>1Tearoom1</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
           <t>Active</t>
@@ -5358,7 +5618,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
           <t>jms@spigener.com</t>
@@ -5396,7 +5655,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -5407,7 +5665,6 @@
           <t>1Tearoom</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
           <t>Active</t>
@@ -5514,7 +5771,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -5594,7 +5850,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -5605,7 +5860,6 @@
           <t>Sycamoreville1</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
           <t>Active</t>
@@ -5628,13 +5882,11 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
           <t>jms@spigener.com</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
           <t>Main email</t>
@@ -5662,7 +5914,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -6036,7 +6287,6 @@
           <t>Booking</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
           <t>admin@silverre</t>
@@ -6047,7 +6297,6 @@
           <t>Silverton</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr">
         <is>
           <t>Active</t>
@@ -6112,7 +6361,6 @@
           <t>Network</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
           <t>admin@silversycamore.com</t>
@@ -6150,7 +6398,6 @@
           <t>Network</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
           <t>Silver Corp</t>
@@ -6198,7 +6445,6 @@
           <t>silverguest</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
           <t>Video conferencing</t>
@@ -6226,7 +6472,6 @@
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
           <t>admin</t>
@@ -6378,8 +6623,6 @@
           <t>Core Team</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>Day-to-day execution, demos</t>
@@ -6417,8 +6660,6 @@
           <t>Core Team</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>Runs catering events, wedding coordination interim</t>
@@ -6456,8 +6697,6 @@
           <t>Core Team</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>Catering events, sales calls</t>
@@ -6485,14 +6724,11 @@
           <t>Part-time</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>Core Team</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
           <t>Supports wedding coordination</t>
@@ -6530,8 +6766,6 @@
           <t>Ownership</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>Friendswood CPA firm</t>
@@ -6559,14 +6793,11 @@
           <t>External</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>Ownership</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>Peterson CPA</t>
@@ -6594,14 +6825,11 @@
           <t>External</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
           <t>Ownership</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>Peterson CPA</t>
@@ -6639,8 +6867,6 @@
           <t>Support</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>Operations consultant</t>
@@ -6668,14 +6894,11 @@
           <t>Exiting (2 weeks)</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
           <t>Legacy</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>Transitioning out</t>
@@ -6703,14 +6926,11 @@
           <t>Exiting (timing TBD)</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>Legacy</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>Function to be automated</t>
@@ -6738,7 +6958,6 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
           <t>Staff</t>
@@ -6749,8 +6968,6 @@
           <t>832-630-5096</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -6773,7 +6990,6 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>Ownership</t>
@@ -6784,8 +7000,6 @@
           <t>281-850-2096</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -6808,7 +7022,6 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
           <t>Ownership</t>
@@ -6819,8 +7032,6 @@
           <t>281-831-0322</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -6843,7 +7054,6 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>Staff</t>
@@ -6854,8 +7064,6 @@
           <t>713-839-5444</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6958,13 +7166,11 @@
           <t>1 (866) 656-8207</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>Booking</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -6987,13 +7193,11 @@
           <t>713-269-8185</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>Linens</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7016,13 +7220,11 @@
           <t>281-460-2141</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>Entertainment</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7045,13 +7247,11 @@
           <t>832-992-1353</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>Cakes</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7074,7 +7274,6 @@
           <t>281-889-1684</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>Cakes</t>
@@ -7107,13 +7306,11 @@
           <t>713-292-7828</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>Rentals</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7136,13 +7333,11 @@
           <t>832-643-7518</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
           <t>Catering</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7175,7 +7370,6 @@
           <t>Signs</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7198,13 +7392,11 @@
           <t>713-907-0733</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
           <t>Catering</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7227,13 +7419,11 @@
           <t>832-272-6610</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>Entertainment</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -7256,13 +7446,11 @@
           <t>713-592-6724</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
           <t>Marketing</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -7285,13 +7473,11 @@
           <t>281-841-2694</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>Food Truck</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -7314,13 +7500,11 @@
           <t>713-671-5294</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -7343,13 +7527,11 @@
           <t>815-263-9716</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>Vendor</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -7372,13 +7554,11 @@
           <t>832-317-8359</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
           <t>Florist</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -7401,13 +7581,11 @@
           <t>832-515-4124</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
           <t>Media</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -7430,13 +7608,11 @@
           <t>281-229-9623</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
           <t>Catering</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -7459,13 +7635,11 @@
           <t>681-620-0742</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
           <t>Entertainment</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -7488,13 +7662,11 @@
           <t>832-423-9788</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -7554,13 +7726,11 @@
           <t>(832) 974-2887</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
           <t>Entertainment</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -7620,13 +7790,11 @@
           <t>713-501-9851</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>Rentals</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -7649,13 +7817,11 @@
           <t>713-690-5857</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
           <t>Linens</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -7678,13 +7844,11 @@
           <t>979-826-8185</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -7707,13 +7871,11 @@
           <t>281-413-3962</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -7736,7 +7898,6 @@
           <t>832-414-0837</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t>Linens</t>
@@ -7769,13 +7930,11 @@
           <t>281-381-5276</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
           <t>Rentals</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -7825,7 +7984,6 @@
           <t>Sycamore Grounds (Officer)</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
           <t>281-978-8307</t>
@@ -7841,7 +7999,6 @@
           <t>Staff</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -7864,7 +8021,6 @@
           <t>409-457-0672</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
           <t>Food Truck</t>
@@ -7887,15 +8043,11 @@
           <t>Republic National</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
           <t>Wine</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -7918,13 +8070,11 @@
           <t>281-728-7531</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
           <t>Wine</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -7947,13 +8097,11 @@
           <t>713-941-3657</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -7976,13 +8124,11 @@
           <t>409-978-5279</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
           <t>Vendor</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -8005,13 +8151,11 @@
           <t>832-630-5096</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
           <t>Staff</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -8034,13 +8178,11 @@
           <t>281-850-2096</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
           <t>Owner</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -8063,13 +8205,11 @@
           <t>281-831-0322</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
           <t>Owner</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -8092,13 +8232,11 @@
           <t>713-839-5444</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
           <t>Staff</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -8121,13 +8259,11 @@
           <t>1-855-627-7594</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
           <t>Rentals</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -8150,13 +8286,11 @@
           <t>281-888-7471</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
           <t>Staff</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -8169,19 +8303,16 @@
           <t>Sysco</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
           <t>713-775-5349</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
           <t>Food Supply</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -8204,7 +8335,6 @@
           <t>713-416-2678</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
           <t>Food Truck</t>
@@ -8237,13 +8367,11 @@
           <t>281-338-9898</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
           <t>Rentals</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -8266,13 +8394,11 @@
           <t>713-410-5466</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
           <t>Security</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -8285,19 +8411,16 @@
           <t>Lonestar</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
           <t>713-926-8100</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
           <t>Services</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -8310,19 +8433,16 @@
           <t>Sterling Tea</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
           <t>972-722-0506</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
           <t>Catering</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8464,7 +8584,6 @@
           <t>Micro Wedding, Reception, Shower, Corporate</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8625,7 +8744,6 @@
           <t>Ceremony</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8654,7 +8772,6 @@
           <t>Ceremony</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8973,7 +9090,6 @@
           <t>calendly.com</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9043,7 +9159,6 @@
           <t>constantcontact.com</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9187,7 +9302,6 @@
           <t>bedandbreakfast.com</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -9220,7 +9334,6 @@
           <t>theknot.com</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -9253,7 +9366,6 @@
           <t>weddingwire.com</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -9286,7 +9398,6 @@
           <t>calendar.google.com</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -9319,7 +9430,6 @@
           <t>dropbox.com</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -9337,7 +9447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9353,6 +9463,7 @@
     <col width="10" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="45" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9412,6 +9523,16 @@
           <t>Deposit</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="J3" s="6" t="inlineStr">
+        <is>
+          <t>What's Included</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9421,28 +9542,38 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Saloon &amp; Town Merry</t>
+          <t>Dream Package</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3200</v>
+        <v>12900</v>
       </c>
       <c r="D4" t="n">
-        <v>4200</v>
+        <v>12900</v>
       </c>
       <c r="E4" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5 hrs</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>20</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2.5 hrs</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>35</v>
-      </c>
       <c r="H4" t="n">
-        <v>1500</v>
+        <v>2000</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ceremony + Reception</t>
+        </is>
+      </c>
+      <c r="J4" s="7" t="inlineStr">
+        <is>
+          <t>Ceremony spaces (White Chapel, Waterfall Gazebo), Reception hall, Bridal cottage, Jail/groom prep, 5-hour rental</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -9476,6 +9607,16 @@
       <c r="H5" t="n">
         <v>2000</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Weekday/Weekend pricing</t>
+        </is>
+      </c>
+      <c r="J5" s="7" t="inlineStr">
+        <is>
+          <t>Ceremony + Reception, Smaller capacity, More intimate setting, 3.5-hour rental</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9485,14 +9626,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Food Truck Fun</t>
+          <t>Reception Only</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10000</v>
+        <v>11400</v>
       </c>
       <c r="D6" t="n">
-        <v>10000</v>
+        <v>11400</v>
       </c>
       <c r="E6" t="n">
         <v>100</v>
@@ -9503,11 +9644,21 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H6" t="n">
         <v>2000</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Reception only</t>
+        </is>
+      </c>
+      <c r="J6" s="7" t="inlineStr">
+        <is>
+          <t>Reception hall only, No ceremony included, 4-hour rental</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9517,92 +9668,38 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dream Package</t>
+          <t>Micro Wedding (Saloon &amp; Town Merry)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>12900</v>
+        <v>3200</v>
       </c>
       <c r="D7" t="n">
-        <v>12900</v>
+        <v>4200</v>
       </c>
       <c r="E7" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5 hrs</t>
+          <t>2.5 hrs</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H7" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>WED-005</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Diamond Package</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>16500</v>
-      </c>
-      <c r="D8" t="n">
-        <v>16500</v>
-      </c>
-      <c r="E8" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>5 hrs</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>35</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>WED-006</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Reception Only</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>11400</v>
-      </c>
-      <c r="D9" t="n">
-        <v>11400</v>
-      </c>
-      <c r="E9" t="n">
-        <v>100</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>4 hrs</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>20</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2000</v>
+        <v>1500</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Small intimate weddings</t>
+        </is>
+      </c>
+      <c r="J7" s="7" t="inlineStr">
+        <is>
+          <t>Saloon &amp; Town spaces, Smallest capacity, Perfect for intimate gatherings, 2.5-hour rental</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -10046,7 +10143,6 @@
       <c r="C13" t="n">
         <v>3000</v>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
         <v>0</v>
       </c>
@@ -10079,7 +10175,6 @@
       <c r="C14" t="n">
         <v>2115</v>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>0</v>
       </c>
@@ -10109,7 +10204,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10185,7 +10280,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Pasta focus</t>
+          <t>Pasta focus with multiple options</t>
         </is>
       </c>
     </row>
@@ -10210,7 +10305,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Chicken entrees</t>
+          <t>Chicken entrees with sides</t>
         </is>
       </c>
     </row>
@@ -10260,7 +10355,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Fajitas + queso fountain</t>
+          <t>Fajitas + queso fountain included</t>
         </is>
       </c>
     </row>
@@ -10310,82 +10405,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Two entree selections</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>CAT-007</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Howdy Partner</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>24.95</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Buffet</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Burgers, casual</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>CAT-008</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Appetizer Menu</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>21.95</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Self-serve buffet</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Acrylic dinnerware</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>CAT-009</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Formal Dinner</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Buffet/Plated</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>China/silver service, $32-45 range</t>
+          <t>Two entree selections, highest tier</t>
         </is>
       </c>
     </row>

</xml_diff>